<commit_message>
Added pull request test to new_environments_sim.py
</commit_message>
<xml_diff>
--- a/ecoli/experiments/new_environments_test/done.xlsx
+++ b/ecoli/experiments/new_environments_test/done.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timjing/Documents/vivarium-ecoli/ecoli/experiments/new_environments_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C792167-5D8B-1B4D-A496-16141AD82CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0E14FC-8AD2-BD4B-BC22-47D41CA5E171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="164">
   <si>
     <t>Environment</t>
   </si>
@@ -608,6 +608,9 @@
   </si>
   <si>
     <t>Psicoselysine_Transport_(Carbon_Source)</t>
+  </si>
+  <si>
+    <t>CONTROL</t>
   </si>
 </sst>
 </file>
@@ -1092,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1938,8 +1941,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="2"/>
+    <row r="76" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>163</v>
+      </c>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>

</xml_diff>